<commit_message>
added Verify ENTER ACCOUNT INFORMATION header is visible test
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/dynamicdata.xlsx
+++ b/src/test/resources/Testdata/dynamicdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{143EB006-41DE-4244-94E0-2AD2B32CEDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{76750EA5-4056-4328-8309-2ECF91B5D3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,12 +12,12 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N25"/>
+  <oleSize ref="A1:J7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>akashmangond6656@gmail.com</t>
   </si>
@@ -145,58 +145,64 @@
     <t>TestUser2</t>
   </si>
   <si>
+    <t>Secret456</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>456 Second Ave</t>
+  </si>
+  <si>
+    <t>Suite 200</t>
+  </si>
+  <si>
+    <t>M5H 2N2</t>
+  </si>
+  <si>
+    <t>TestUser3</t>
+  </si>
+  <si>
+    <t>MyPass789</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>GlobalInc</t>
+  </si>
+  <si>
+    <t>789 Third Blvd</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>Melbourne</t>
+  </si>
+  <si>
+    <t>NrXqTP9VxF@Yt</t>
+  </si>
+  <si>
+    <t>user3_@example.com</t>
+  </si>
+  <si>
+    <t>user2_@example.com</t>
+  </si>
+  <si>
     <t>user2_{{unique}}@example.com</t>
   </si>
   <si>
-    <t>Secret456</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>456 Second Ave</t>
-  </si>
-  <si>
-    <t>Suite 200</t>
-  </si>
-  <si>
-    <t>M5H 2N2</t>
-  </si>
-  <si>
-    <t>TestUser3</t>
-  </si>
-  <si>
     <t>user3_{{unique}}@example.com</t>
-  </si>
-  <si>
-    <t>MyPass789</t>
-  </si>
-  <si>
-    <t>January</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Williams</t>
-  </si>
-  <si>
-    <t>GlobalInc</t>
-  </si>
-  <si>
-    <t>789 Third Blvd</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Victoria</t>
-  </si>
-  <si>
-    <t>Melbourne</t>
-  </si>
-  <si>
-    <t>NrXqTP9VxF@Yt</t>
   </si>
 </sst>
 </file>
@@ -581,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="106" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,21 +610,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{6F717537-93B7-41F9-9464-9DE7564F767B}"/>
     <hyperlink ref="A1" r:id="rId2" display="akashmangond6656@gmail.com" xr:uid="{5A5342D1-097B-4602-A241-16F8B24A8C55}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{ED067260-1098-4684-9441-D92DB6E5BE7E}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{88C5696D-AA61-480F-989D-815066E032D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -628,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9460CC0-D0FE-416A-8C3D-F79F1A99F49B}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,11 +774,11 @@
       <c r="A3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
         <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
       </c>
       <c r="D3">
         <v>25</v>
@@ -774,10 +790,10 @@
         <v>1990</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -789,10 +805,10 @@
         <v>22</v>
       </c>
       <c r="L3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" t="s">
         <v>45</v>
-      </c>
-      <c r="M3" t="s">
-        <v>46</v>
       </c>
       <c r="N3" t="s">
         <v>17</v>
@@ -804,7 +820,7 @@
         <v>19</v>
       </c>
       <c r="Q3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R3">
         <v>14165550123</v>
@@ -812,25 +828,25 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
         <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
       </c>
       <c r="D4">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F4">
         <v>2000</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -839,22 +855,22 @@
         <v>26</v>
       </c>
       <c r="J4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" t="s">
         <v>53</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>54</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>55</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>56</v>
-      </c>
-      <c r="O4" t="s">
-        <v>57</v>
-      </c>
-      <c r="P4" t="s">
-        <v>58</v>
       </c>
       <c r="Q4">
         <v>3000</v>
@@ -864,6 +880,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{E2A4A558-1CC4-4E1D-BA13-7D7E2B18A284}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{C833AEED-0E23-454C-91B4-A4B1FA9E1478}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added click utility and some test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/dynamicdata.xlsx
+++ b/src/test/resources/Testdata/dynamicdata.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D53974E9-A7A7-4093-94B7-05A62E6313B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D35EA1AC-7039-49DF-9E4B-4E8237EF540D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DynamicData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M24"/>
+  <oleSize ref="A1:W22"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>akashmangond6656@gmail.com</t>
   </si>
@@ -193,23 +193,38 @@
     <t>NrXqTP9VxF@Yt</t>
   </si>
   <si>
-    <t>user3_@example.com</t>
-  </si>
-  <si>
-    <t>user2_@example.com</t>
-  </si>
-  <si>
     <t>user2_{{unique}}@example.com</t>
   </si>
   <si>
     <t>user3_{{unique}}@example.com</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>90001</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>14165550123</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>61390123456</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -218,9 +233,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -234,7 +271,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -242,18 +279,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{3A76ADF8-287B-4312-96E7-32313482F5EF}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{7EB4F593-496B-49B4-8263-EA978CD552CA}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -587,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="63" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,44 +662,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{6F717537-93B7-41F9-9464-9DE7564F767B}"/>
-    <hyperlink ref="A1" r:id="rId2" display="akashmangond6656@gmail.com" xr:uid="{5A5342D1-097B-4602-A241-16F8B24A8C55}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{ED067260-1098-4684-9441-D92DB6E5BE7E}"/>
-    <hyperlink ref="A3" r:id="rId4" xr:uid="{88C5696D-AA61-480F-989D-815066E032D9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -644,246 +692,252 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9460CC0-D0FE-416A-8C3D-F79F1A99F49B}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.5546875" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.109375" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>1995</v>
       </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="Q2">
-        <v>90001</v>
-      </c>
-      <c r="R2">
-        <v>1234567890</v>
+      <c r="Q2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>1990</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="R3">
-        <v>14165550123</v>
+      <c r="R3" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>2000</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N4" t="s">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Q4">
-        <v>3000</v>
-      </c>
-      <c r="R4">
-        <v>61390123456</v>
+      <c r="Q4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{E2A4A558-1CC4-4E1D-BA13-7D7E2B18A284}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{C833AEED-0E23-454C-91B4-A4B1FA9E1478}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added contact us test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/dynamicdata.xlsx
+++ b/src/test/resources/Testdata/dynamicdata.xlsx
@@ -2,22 +2,27 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D35EA1AC-7039-49DF-9E4B-4E8237EF540D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91951\Desktop\Automation_Exercise_TEAM_A1\Automation_Exercise_Project\src\test\resources\Testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64162A5C-63BB-48B4-AAF6-4C02FDA221D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DynamicData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="ContactUs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:W22"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
   <si>
     <t>akashmangond6656@gmail.com</t>
   </si>
@@ -218,6 +223,81 @@
   </si>
   <si>
     <t>61390123456</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>expectedMessage</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>john@example.com</t>
+  </si>
+  <si>
+    <t>Test Subject 1</t>
+  </si>
+  <si>
+    <t>This is a test message.</t>
+  </si>
+  <si>
+    <t>Success! Your details have been submitted successfully.</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>jane@example.com</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Loved the website!</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>invalid-email</t>
+  </si>
+  <si>
+    <t>Test Error</t>
+  </si>
+  <si>
+    <t>Missing proper email format.</t>
+  </si>
+  <si>
+    <t>Please enter a valid email address.</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>No Email</t>
+  </si>
+  <si>
+    <t>No email provided.</t>
+  </si>
+  <si>
+    <t>Email is required.</t>
+  </si>
+  <si>
+    <t>Long Text</t>
+  </si>
+  <si>
+    <t>longtext@example.com</t>
+  </si>
+  <si>
+    <t>Test Long</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet...</t>
   </si>
 </sst>
 </file>
@@ -655,13 +735,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -669,7 +749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -677,10 +757,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -692,30 +772,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9460CC0-D0FE-416A-8C3D-F79F1A99F49B}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
+    <sheetView zoomScale="63" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.08984375" customWidth="1"/>
+    <col min="13" max="13" width="15.6328125" customWidth="1"/>
+    <col min="14" max="14" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -771,7 +851,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -827,7 +907,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -883,7 +963,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -935,6 +1015,127 @@
       </c>
       <c r="R4" s="2" t="s">
         <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FCE4BE-1E56-4E4D-A99D-24C890B87186}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.6328125" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="22.08984375" customWidth="1"/>
+    <col min="5" max="5" width="45.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added subscription page and few test cases to contactus
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/dynamicdata.xlsx
+++ b/src/test/resources/Testdata/dynamicdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91951\Desktop\Automation_Exercise_TEAM_A1\Automation_Exercise_Project\src\test\resources\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64162A5C-63BB-48B4-AAF6-4C02FDA221D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FB9141-753A-44BF-8BB4-CBB05C909D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,13 +16,14 @@
     <sheet name="DynamicData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="ContactUs" sheetId="3" r:id="rId3"/>
+    <sheet name="Subscription" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="104">
   <si>
     <t>akashmangond6656@gmail.com</t>
   </si>
@@ -285,9 +286,6 @@
     <t>No email provided.</t>
   </si>
   <si>
-    <t>Email is required.</t>
-  </si>
-  <si>
     <t>Long Text</t>
   </si>
   <si>
@@ -298,13 +296,52 @@
   </si>
   <si>
     <t>Lorem ipsum dolor sit amet...</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>ExpectedMessage</t>
+  </si>
+  <si>
+    <t>valid@example.com</t>
+  </si>
+  <si>
+    <t>You have been successfully subscribed!</t>
+  </si>
+  <si>
+    <t>Please fill out this field</t>
+  </si>
+  <si>
+    <t>invalidemail</t>
+  </si>
+  <si>
+    <t>Please include an '@' in the email address</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>John@123#</t>
+  </si>
+  <si>
+    <t>validemail@example.com</t>
+  </si>
+  <si>
+    <t>Invalid Name TC</t>
+  </si>
+  <si>
+    <t>Testing invalid characters.</t>
+  </si>
+  <si>
+    <t>INVALID_NAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -338,6 +375,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -381,7 +426,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
@@ -391,6 +436,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1024,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FCE4BE-1E56-4E4D-A99D-24C890B87186}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1118,27 +1172,99 @@
         <v>86</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
         <v>88</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>89</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>90</v>
-      </c>
-      <c r="D6" t="s">
-        <v>91</v>
       </c>
       <c r="E6" t="s">
         <v>74</v>
       </c>
     </row>
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" display="mailto:validemail@example.com" xr:uid="{BF3958F5-516A-4300-A227-3A9D7EA30DB6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A3156D-12F5-4419-BF1B-1FCB80B9558E}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="42.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="mailto:valid@example.com" xr:uid="{8E9CFF72-FF36-4A6E-91EB-0D2C378F3E5D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated 2-3 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/dynamicdata.xlsx
+++ b/src/test/resources/Testdata/dynamicdata.xlsx
@@ -1,28 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91951\Desktop\Automation_Exercise_TEAM_A1\Automation_Exercise_Project\src\test\resources\Testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64162A5C-63BB-48B4-AAF6-4C02FDA221D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8893B493-8AE1-4EA8-8D3D-32718C98D9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DynamicData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="ContactUs" sheetId="3" r:id="rId3"/>
+    <sheet name="InvalidLoginData" sheetId="4" r:id="rId3"/>
+    <sheet name="InvalidEmailData" sheetId="5" r:id="rId4"/>
+    <sheet name="ContactUs" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:Q25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="100">
   <si>
     <t>akashmangond6656@gmail.com</t>
   </si>
@@ -298,16 +296,47 @@
   </si>
   <si>
     <t>Lorem ipsum dolor sit amet...</t>
+  </si>
+  <si>
+    <t>fakeuser@example.com</t>
+  </si>
+  <si>
+    <t>wrongPassword123</t>
+  </si>
+  <si>
+    <t>expectedError</t>
+  </si>
+  <si>
+    <t>Your email or password is incorrect!</t>
+  </si>
+  <si>
+    <t>plainaddress</t>
+  </si>
+  <si>
+    <t>include an '@'</t>
+  </si>
+  <si>
+    <t>invalidEmail</t>
+  </si>
+  <si>
+    <t>expectedValidation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -375,29 +404,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{3A76ADF8-287B-4312-96E7-32313482F5EF}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{7EB4F593-496B-49B4-8263-EA978CD552CA}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{ADB137B8-E7EB-4606-9233-47929ACCC98C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -731,17 +766,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="63" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -749,7 +784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -757,10 +792,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -770,32 +805,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9460CC0-D0FE-416A-8C3D-F79F1A99F49B}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView zoomScale="63" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.08984375" customWidth="1"/>
-    <col min="13" max="13" width="15.6328125" customWidth="1"/>
-    <col min="14" max="14" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -851,7 +886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -907,7 +942,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -963,7 +998,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -1016,6 +1051,106 @@
       <c r="R4" s="2" t="s">
         <v>66</v>
       </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1023,23 +1158,116 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49B245BF-6E18-4BBF-A09C-82B6FEDFDB1A}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E9A61E82-19E0-4D51-8736-490AF6C29B37}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BF1878-1B18-4F47-9319-02580F9E35FD}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FCE4BE-1E56-4E4D-A99D-24C890B87186}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6328125" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" customWidth="1"/>
-    <col min="5" max="5" width="45.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="45.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1056,7 +1284,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1073,7 +1301,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1090,7 +1318,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -1107,7 +1335,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -1121,7 +1349,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Added a row in dynamic data
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/dynamicdata.xlsx
+++ b/src/test/resources/Testdata/dynamicdata.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C2E0AE00-548C-47C8-A249-BC2983A28073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91951\Desktop\Automation_Exercise_TEAM_A1\Automation_Exercise_Project\src\test\resources\Testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CF113C-C324-4E65-8C29-47EFBA2113B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="742" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="742" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DynamicData" sheetId="1" r:id="rId1"/>
@@ -16,12 +21,11 @@
     <sheet name="ContactUs" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="112">
   <si>
     <t>akashmangond6656@gmail.com</t>
   </si>
@@ -342,6 +346,21 @@
   </si>
   <si>
     <t>Please include an '@' in the email address</t>
+  </si>
+  <si>
+    <t>John@123#</t>
+  </si>
+  <si>
+    <t>validemail@example.com</t>
+  </si>
+  <si>
+    <t>Invalid Name TC</t>
+  </si>
+  <si>
+    <t>Testing invalid characters.</t>
+  </si>
+  <si>
+    <t>INVALID_NAME</t>
   </si>
 </sst>
 </file>
@@ -792,13 +811,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -806,7 +825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -814,10 +833,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -829,17 +848,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14F265F-8F65-4E50-B457-62460B134BC3}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -847,7 +866,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
@@ -855,12 +874,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -884,26 +903,26 @@
       <selection activeCell="N5" sqref="N5:R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.08984375" customWidth="1"/>
+    <col min="13" max="13" width="15.6328125" customWidth="1"/>
+    <col min="14" max="14" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -959,7 +978,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -1015,7 +1034,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -1071,7 +1090,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -1125,7 +1144,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1145,7 +1164,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1165,7 +1184,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1185,7 +1204,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1205,7 +1224,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1238,14 +1257,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1256,7 +1275,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -1283,14 +1302,14 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1301,7 +1320,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
@@ -1312,10 +1331,10 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
     </row>
   </sheetData>
@@ -1325,22 +1344,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FCE4BE-1E56-4E4D-A99D-24C890B87186}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.6328125" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="45.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.08984375" customWidth="1"/>
+    <col min="5" max="5" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1357,7 +1376,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1374,7 +1393,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1391,7 +1410,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -1408,7 +1427,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -1422,7 +1441,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -1437,6 +1456,23 @@
       </c>
       <c r="E6" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated some bugs test cases in registration page
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/dynamicdata.xlsx
+++ b/src/test/resources/Testdata/dynamicdata.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91951\Desktop\Automation_Exercise_TEAM_A1\Automation_Exercise_Project\src\test\resources\Testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CF113C-C324-4E65-8C29-47EFBA2113B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{83293DA9-DBB1-4F06-B333-5F48C3ABE604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="742" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="742" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DynamicData" sheetId="1" r:id="rId1"/>
@@ -19,13 +14,15 @@
     <sheet name="InvalidLoginData" sheetId="4" r:id="rId4"/>
     <sheet name="InvalidEmailData" sheetId="5" r:id="rId5"/>
     <sheet name="ContactUs" sheetId="3" r:id="rId6"/>
+    <sheet name="RegistrationRequiredFields" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:M25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="121">
   <si>
     <t>akashmangond6656@gmail.com</t>
   </si>
@@ -361,16 +358,50 @@
   </si>
   <si>
     <t>INVALID_NAME</t>
+  </si>
+  <si>
+    <t>TempUser</t>
+  </si>
+  <si>
+    <t>reg_req_{{unique}}@ex.com</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>123 Street</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>M1A1A1</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>Test1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -445,35 +476,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{3A76ADF8-287B-4312-96E7-32313482F5EF}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{7EB4F593-496B-49B4-8263-EA978CD552CA}"/>
     <cellStyle name="Normal 4" xfId="4" xr:uid="{ADB137B8-E7EB-4606-9233-47929ACCC98C}"/>
+    <cellStyle name="Normal 5" xfId="5" xr:uid="{E48D672B-2254-4E89-9C80-BF5D03EF837E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -808,16 +842,16 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -825,7 +859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -833,10 +867,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -852,13 +886,13 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -866,7 +900,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
@@ -874,12 +908,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -899,30 +933,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9460CC0-D0FE-416A-8C3D-F79F1A99F49B}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N5" sqref="N5:R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.08984375" customWidth="1"/>
-    <col min="13" max="13" width="15.6328125" customWidth="1"/>
-    <col min="14" max="14" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -978,7 +1012,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -1034,7 +1068,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -1090,7 +1124,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
@@ -1144,7 +1178,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1164,7 +1198,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1184,7 +1218,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1204,7 +1238,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1224,7 +1258,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1257,14 +1291,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1275,7 +1309,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -1302,14 +1336,14 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.90625" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1320,7 +1354,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
@@ -1331,10 +1365,10 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
     </row>
   </sheetData>
@@ -1346,20 +1380,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FCE4BE-1E56-4E4D-A99D-24C890B87186}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6328125" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" customWidth="1"/>
-    <col min="5" max="5" width="45.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="45.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1376,7 +1410,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1393,7 +1427,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1410,7 +1444,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -1427,7 +1461,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -1441,7 +1475,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -1458,7 +1492,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>107</v>
       </c>
@@ -1474,6 +1508,360 @@
       <c r="E7" t="s">
         <v>111</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71ADD0A6-ADF9-43A4-B0CF-0A9EC37ED200}">
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cart and Payment page
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/dynamicdata.xlsx
+++ b/src/test/resources/Testdata/dynamicdata.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{76750EA5-4056-4328-8309-2ECF91B5D3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{611C3FC3-0B11-4EBC-BB0A-983B39D83054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DynamicData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="ContactUs" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
+    <sheet name="Payment" sheetId="6" r:id="rId5"/>
+    <sheet name="Subscription" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J7"/>
+  <oleSize ref="A1:M13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="121">
   <si>
     <t>akashmangond6656@gmail.com</t>
   </si>
@@ -193,23 +197,200 @@
     <t>NrXqTP9VxF@Yt</t>
   </si>
   <si>
-    <t>user3_@example.com</t>
-  </si>
-  <si>
-    <t>user2_@example.com</t>
-  </si>
-  <si>
     <t>user2_{{unique}}@example.com</t>
   </si>
   <si>
     <t>user3_{{unique}}@example.com</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>90001</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>14165550123</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>61390123456</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>expectedMessage</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>john@example.com</t>
+  </si>
+  <si>
+    <t>Test Subject 1</t>
+  </si>
+  <si>
+    <t>This is a test message.</t>
+  </si>
+  <si>
+    <t>Success! Your details have been submitted successfully.</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>jane@example.com</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Loved the website!</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>invalid-email</t>
+  </si>
+  <si>
+    <t>Test Error</t>
+  </si>
+  <si>
+    <t>Missing proper email format.</t>
+  </si>
+  <si>
+    <t>Please enter a valid email address.</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>No Email</t>
+  </si>
+  <si>
+    <t>No email provided.</t>
+  </si>
+  <si>
+    <t>Long Text</t>
+  </si>
+  <si>
+    <t>longtext@example.com</t>
+  </si>
+  <si>
+    <t>Test Long</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet...</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>ExpectedMessage</t>
+  </si>
+  <si>
+    <t>valid@example.com</t>
+  </si>
+  <si>
+    <t>You have been successfully subscribed!</t>
+  </si>
+  <si>
+    <t>Please fill out this field</t>
+  </si>
+  <si>
+    <t>invalidemail</t>
+  </si>
+  <si>
+    <t>Please include an '@' in the email address</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>John@123#</t>
+  </si>
+  <si>
+    <t>validemail@example.com</t>
+  </si>
+  <si>
+    <t>Invalid Name TC</t>
+  </si>
+  <si>
+    <t>Testing invalid characters.</t>
+  </si>
+  <si>
+    <t>INVALID_NAME</t>
+  </si>
+  <si>
+    <t>ProductId</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Blue Top</t>
+  </si>
+  <si>
+    <t>Men Tshirt</t>
+  </si>
+  <si>
+    <t>vasudhaktippari26@gmail.com</t>
+  </si>
+  <si>
+    <t>vasu@123</t>
+  </si>
+  <si>
+    <t>vasu@124</t>
+  </si>
+  <si>
+    <t>NameOnCard</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>CVC</t>
+  </si>
+  <si>
+    <t>ExpMonth</t>
+  </si>
+  <si>
+    <t>ExpYear</t>
+  </si>
+  <si>
+    <t>Vasudha</t>
+  </si>
+  <si>
+    <t>Test123</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>20ab</t>
+  </si>
+  <si>
+    <t>(blank)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -218,9 +399,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -234,7 +451,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -242,18 +459,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{3A76ADF8-287B-4312-96E7-32313482F5EF}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{7EB4F593-496B-49B4-8263-EA978CD552CA}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -587,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="106" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="63" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,44 +851,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{6F717537-93B7-41F9-9464-9DE7564F767B}"/>
-    <hyperlink ref="A1" r:id="rId2" display="akashmangond6656@gmail.com" xr:uid="{5A5342D1-097B-4602-A241-16F8B24A8C55}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{ED067260-1098-4684-9441-D92DB6E5BE7E}"/>
-    <hyperlink ref="A3" r:id="rId4" xr:uid="{88C5696D-AA61-480F-989D-815066E032D9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -644,21 +881,274 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9460CC0-D0FE-416A-8C3D-F79F1A99F49B}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="63" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.5546875" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.109375" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1995</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1990</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2000</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FCE4BE-1E56-4E4D-A99D-24C890B87186}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="45.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -666,223 +1156,320 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2">
-        <v>1995</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2">
-        <v>90001</v>
-      </c>
-      <c r="R2">
-        <v>1234567890</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3">
-        <v>25</v>
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3">
-        <v>1990</v>
-      </c>
-      <c r="G3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3">
-        <v>14165550123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4">
-        <v>2000</v>
-      </c>
-      <c r="G4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" t="s">
-        <v>54</v>
-      </c>
-      <c r="O4" t="s">
-        <v>55</v>
-      </c>
-      <c r="P4" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q4">
-        <v>3000</v>
-      </c>
-      <c r="R4">
-        <v>61390123456</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{E2A4A558-1CC4-4E1D-BA13-7D7E2B18A284}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{C833AEED-0E23-454C-91B4-A4B1FA9E1478}"/>
+    <hyperlink ref="B7" r:id="rId1" display="mailto:validemail@example.com" xr:uid="{BF3958F5-516A-4300-A227-3A9D7EA30DB6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF59B04-C3F7-4891-986F-9E094CA61387}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4EDF9538-C595-4C93-802A-AB44627CB9F9}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{1CADE6CA-B338-421D-8E78-DFA9C2C90187}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{CC09CED7-A048-4BEA-8149-FE69175133A8}"/>
+    <hyperlink ref="B3" r:id="rId4" display="vasu@123" xr:uid="{C18DF802-A508-4C74-8FE6-918B6BABF265}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E348FF-BE1C-4490-BC9F-1D7C2084AD6E}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1234567890123450</v>
+      </c>
+      <c r="C2" s="7">
+        <v>123</v>
+      </c>
+      <c r="D2" s="7">
+        <v>12</v>
+      </c>
+      <c r="E2" s="7">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="7">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7">
+        <v>15</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1111222233334440</v>
+      </c>
+      <c r="C4" s="7">
+        <v>321</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>2028</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A3156D-12F5-4419-BF1B-1FCB80B9558E}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="mailto:valid@example.com" xr:uid="{8E9CFF72-FF36-4A6E-91EB-0D2C378F3E5D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>